<commit_message>
Documentação Controle de Relatórios
</commit_message>
<xml_diff>
--- a/Relatórios LN/Controle_Relatorios.xlsx
+++ b/Relatórios LN/Controle_Relatorios.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3704" uniqueCount="721">
   <si>
     <t>Relatório</t>
   </si>
@@ -2146,6 +2146,39 @@
   </si>
   <si>
     <t>LN_MarketPlace_RelatorioPedidosPAPMarketPlace</t>
+  </si>
+  <si>
+    <t>LN_Contabilidade_RelatorioPedidosIntegrados</t>
+  </si>
+  <si>
+    <t>LN_Fiscal_RelatorioPedidosInternos</t>
+  </si>
+  <si>
+    <t>LN_Contabilidade_RelatorioPedidosMarketPlace</t>
+  </si>
+  <si>
+    <t>LN_TI_RelatorioPedidosStatusPAP</t>
+  </si>
+  <si>
+    <t>LN_Transp_RelatorioPLCorreioDimensoes_eHub</t>
+  </si>
+  <si>
+    <t>LN_Supply_RelatorioPreRecebimentoConsignacao</t>
+  </si>
+  <si>
+    <t>LN_Supply_RelatorioPreRecebimentoConsignacao_Ehub</t>
+  </si>
+  <si>
+    <t>LN_Transp_RelatorioQRY0450PedidoExpedidoDataTransporteDocaCompleto</t>
+  </si>
+  <si>
+    <t>LN_Transp_RelatorioQRY0450PedidoExpedidoDataTransporteDocaCompleto_eHub</t>
+  </si>
+  <si>
+    <t>LN_Supply_RelatorioRascunhoXLM</t>
+  </si>
+  <si>
+    <t>LN_Supply_RelatorioRascunhoXLM-eHub</t>
   </si>
 </sst>
 </file>
@@ -6903,8 +6936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD93"/>
     </sheetView>
   </sheetViews>
@@ -8812,8 +8845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C131" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -8823,7 +8856,7 @@
     <col min="3" max="3" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="101.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="57.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="66.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="7"/>
@@ -11852,6 +11885,9 @@
       <c r="E129" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="F129" s="7" t="s">
+        <v>710</v>
+      </c>
       <c r="G129" s="7" t="s">
         <v>23</v>
       </c>
@@ -11872,6 +11908,9 @@
       <c r="E130" s="7" t="s">
         <v>121</v>
       </c>
+      <c r="F130" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="G130" s="7" t="s">
         <v>122</v>
       </c>
@@ -11892,6 +11931,9 @@
       <c r="E131" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="F131" s="7" t="s">
+        <v>712</v>
+      </c>
       <c r="G131" s="7" t="s">
         <v>25</v>
       </c>
@@ -11912,6 +11954,9 @@
       <c r="E132" s="7" t="s">
         <v>357</v>
       </c>
+      <c r="F132" s="7" t="s">
+        <v>713</v>
+      </c>
       <c r="G132" s="7" t="s">
         <v>359</v>
       </c>
@@ -11932,6 +11977,9 @@
       <c r="E133" s="7" t="s">
         <v>532</v>
       </c>
+      <c r="F133" s="7" t="s">
+        <v>714</v>
+      </c>
       <c r="G133" s="7" t="s">
         <v>533</v>
       </c>
@@ -11952,6 +12000,9 @@
       <c r="E134" s="7" t="s">
         <v>339</v>
       </c>
+      <c r="F134" s="7" t="s">
+        <v>715</v>
+      </c>
       <c r="G134" s="7" t="s">
         <v>340</v>
       </c>
@@ -11972,6 +12023,9 @@
       <c r="E135" s="7" t="s">
         <v>518</v>
       </c>
+      <c r="F135" s="7" t="s">
+        <v>716</v>
+      </c>
       <c r="G135" s="7" t="s">
         <v>340</v>
       </c>
@@ -11995,6 +12049,9 @@
       <c r="E136" s="7" t="s">
         <v>398</v>
       </c>
+      <c r="F136" s="7" t="s">
+        <v>717</v>
+      </c>
       <c r="G136" s="7" t="s">
         <v>399</v>
       </c>
@@ -12015,6 +12072,9 @@
       <c r="E137" s="7" t="s">
         <v>534</v>
       </c>
+      <c r="F137" s="7" t="s">
+        <v>718</v>
+      </c>
       <c r="G137" s="7" t="s">
         <v>399</v>
       </c>
@@ -12035,6 +12095,9 @@
       <c r="E138" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="F138" s="7" t="s">
+        <v>719</v>
+      </c>
       <c r="G138" s="7" t="s">
         <v>342</v>
       </c>
@@ -12054,6 +12117,9 @@
       </c>
       <c r="E139" s="7" t="s">
         <v>519</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>720</v>
       </c>
       <c r="G139" s="7" t="s">
         <v>342</v>

</xml_diff>